<commit_message>
se esta realizando la clase 2 de aplicadas 2
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/clase_1/practica_1.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/clase_1/practica_1.xlsx
@@ -12,27 +12,34 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="edades">Hoja1!$D$6:$D$8</definedName>
     <definedName name="mirango">Hoja1!#REF!</definedName>
     <definedName name="notas">Hoja1!#REF!</definedName>
-    <definedName name="rango_notas">Hoja1!$D$4:$D$5</definedName>
+    <definedName name="rango_notas">Hoja1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>alumno 1</t>
-  </si>
-  <si>
-    <t>alumno 2</t>
-  </si>
-  <si>
-    <t>notas</t>
-  </si>
-  <si>
-    <t>total</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>CRIOLLO GARCIA JESSICA VIVIANA</t>
+  </si>
+  <si>
+    <t>ECHEVERRIA MOREIRA GIOVANNI JAVIER</t>
+  </si>
+  <si>
+    <t>ERAZO LAVAYEN ERIKA LISBETH</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Suma</t>
   </si>
 </sst>
 </file>
@@ -74,7 +81,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -371,49 +400,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D6"/>
+  <dimension ref="C5:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f>SUM(rango_notas)</f>
-        <v>11</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f>SUM(edades)</f>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:D8">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D6&lt;25</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>